<commit_message>
small typo and added file Close() handler so that when executed getAllContent(), Can still updateFile() afterward without refreshing.
</commit_message>
<xml_diff>
--- a/Back-end/src/main/resources/ElectionCourse/kv-lijst.xlsx
+++ b/Back-end/src/main/resources/ElectionCourse/kv-lijst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guanh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CAA800-0909-49F2-B3C6-C066BDA1083D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3243B8B7-A887-4B24-8278-381E8203F59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34110" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roosterinformatie" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2255,13 +2255,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J210"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2275,7 +2275,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>284</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>314</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>314</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>316</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>316</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>316</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>317</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>317</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>318</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>318</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>318</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>319</v>
       </c>
@@ -2629,7 +2629,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>320</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>320</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="21" customHeight="1">
+    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>321</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1">
+    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>321</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>322</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>323</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>325</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="21" customHeight="1">
+    <row r="20" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>326</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>329</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>329</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>331</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="21" customHeight="1">
+    <row r="24" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>332</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>292</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>1</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>1</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>1</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>8</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>293</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>32</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>32</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="21" customHeight="1">
+    <row r="35" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="21" customHeight="1">
+    <row r="36" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>48</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="21" customHeight="1">
+    <row r="37" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>52</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="21" customHeight="1">
+    <row r="38" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>341</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>341</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>59</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="21" customHeight="1">
+    <row r="43" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>62</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="21" customHeight="1">
+    <row r="44" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>66</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>69</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>72</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>74</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>76</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="21" customHeight="1">
+    <row r="49" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>79</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>82</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="21" customHeight="1">
+    <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>84</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>86</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>301</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>89</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>91</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>94</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>97</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>353</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>353</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>101</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>101</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>104</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="21" customHeight="1">
+    <row r="63" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>356</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>359</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>108</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>108</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>111</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>115</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>115</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>115</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>115</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>118</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="21" customHeight="1">
+    <row r="73" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>121</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>304</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>124</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>124</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>124</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>124</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>362</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="21" customHeight="1">
+    <row r="80" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>126</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="21" customHeight="1">
+    <row r="81" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>126</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="21" customHeight="1">
+    <row r="82" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>126</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="21" customHeight="1">
+    <row r="83" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>365</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>130</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>130</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="21" customHeight="1">
+    <row r="86" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>133</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>136</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>139</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="21" customHeight="1">
+    <row r="89" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>141</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="21" customHeight="1">
+    <row r="90" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>141</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="21" customHeight="1">
+    <row r="91" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>141</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="21" customHeight="1">
+    <row r="92" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>141</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="21" customHeight="1">
+    <row r="93" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>144</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="21" customHeight="1">
+    <row r="94" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>144</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="21" customHeight="1">
+    <row r="95" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>144</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="21" customHeight="1">
+    <row r="96" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>144</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>145</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>145</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>148</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>152</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>154</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>371</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15" customHeight="1">
+    <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>374</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="15" customHeight="1">
+    <row r="104" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>157</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>160</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>160</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1">
+    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>163</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>376</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>379</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
         <v>165</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="21" customHeight="1">
+    <row r="111" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
         <v>383</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="21" customHeight="1">
+    <row r="112" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
         <v>383</v>
       </c>
@@ -5781,7 +5781,7 @@
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
     </row>
-    <row r="113" spans="1:10" ht="21" customHeight="1">
+    <row r="113" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>307</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
         <v>387</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="21" customHeight="1">
+    <row r="115" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
         <v>167</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="21" customHeight="1">
+    <row r="116" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
         <v>167</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>392</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="21" customHeight="1">
+    <row r="118" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>395</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
         <v>398</v>
       </c>
@@ -5987,7 +5987,7 @@
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
         <v>400</v>
       </c>
@@ -6013,7 +6013,7 @@
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>400</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>400</v>
       </c>
@@ -6065,7 +6065,7 @@
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
         <v>400</v>
       </c>
@@ -6091,7 +6091,7 @@
       <c r="I123" s="15"/>
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="1:10" ht="21" customHeight="1">
+    <row r="124" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
         <v>169</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="21" customHeight="1">
+    <row r="125" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>169</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="21" customHeight="1">
+    <row r="126" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>169</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="21" customHeight="1">
+    <row r="127" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>402</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="21" customHeight="1">
+    <row r="128" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
         <v>402</v>
       </c>
@@ -6237,7 +6237,7 @@
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
         <v>176</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>179</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="21" customHeight="1">
+    <row r="131" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>183</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>404</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
         <v>187</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="6" t="s">
         <v>191</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>195</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>195</v>
       </c>
@@ -6479,7 +6479,7 @@
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
     </row>
-    <row r="137" spans="1:10" ht="21" customHeight="1">
+    <row r="137" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>406</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>198</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>198</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>198</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>198</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>198</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>202</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="21" customHeight="1">
+    <row r="144" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>204</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="21" customHeight="1">
+    <row r="145" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>204</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="21" customHeight="1">
+    <row r="146" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>208</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="21" customHeight="1">
+    <row r="147" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>208</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="21" customHeight="1">
+    <row r="148" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>208</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>213</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>213</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>213</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>213</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>213</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
         <v>213</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
         <v>218</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>218</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>221</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
         <v>225</v>
       </c>
@@ -7169,7 +7169,7 @@
       <c r="I158" s="15"/>
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="1:10" ht="21" customHeight="1">
+    <row r="159" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="11" t="s">
         <v>227</v>
       </c>
@@ -7197,7 +7197,7 @@
       <c r="I159" s="15"/>
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
         <v>230</v>
       </c>
@@ -7225,7 +7225,7 @@
       <c r="I160" s="15"/>
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
         <v>233</v>
       </c>
@@ -7253,7 +7253,7 @@
       <c r="I161" s="15"/>
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="1:10" ht="21" customHeight="1">
+    <row r="162" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
         <v>235</v>
       </c>
@@ -7281,7 +7281,7 @@
       <c r="I162" s="15"/>
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
         <v>237</v>
       </c>
@@ -7309,7 +7309,7 @@
       <c r="I163" s="15"/>
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="1:10" ht="21" customHeight="1">
+    <row r="164" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
         <v>415</v>
       </c>
@@ -7337,7 +7337,7 @@
       <c r="I164" s="15"/>
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
         <v>240</v>
       </c>
@@ -7365,7 +7365,7 @@
       <c r="I165" s="15"/>
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
         <v>243</v>
       </c>
@@ -7393,7 +7393,7 @@
       <c r="I166" s="15"/>
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
         <v>243</v>
       </c>
@@ -7421,7 +7421,7 @@
       <c r="I167" s="15"/>
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="11" t="s">
         <v>246</v>
       </c>
@@ -7449,7 +7449,7 @@
       <c r="I168" s="15"/>
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
         <v>248</v>
       </c>
@@ -7477,7 +7477,7 @@
       <c r="I169" s="15"/>
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
         <v>251</v>
       </c>
@@ -7503,7 +7503,7 @@
       <c r="I170" s="15"/>
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
         <v>253</v>
       </c>
@@ -7531,7 +7531,7 @@
       <c r="I171" s="15"/>
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
         <v>309</v>
       </c>
@@ -7557,7 +7557,7 @@
       <c r="I172" s="15"/>
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
         <v>256</v>
       </c>
@@ -7585,7 +7585,7 @@
       <c r="I173" s="15"/>
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
         <v>256</v>
       </c>
@@ -7613,7 +7613,7 @@
       <c r="I174" s="15"/>
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
         <v>256</v>
       </c>
@@ -7641,7 +7641,7 @@
       <c r="I175" s="15"/>
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
         <v>256</v>
       </c>
@@ -7669,7 +7669,7 @@
       <c r="I176" s="15"/>
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
         <v>256</v>
       </c>
@@ -7697,7 +7697,7 @@
       <c r="I177" s="15"/>
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
         <v>256</v>
       </c>
@@ -7725,7 +7725,7 @@
       <c r="I178" s="15"/>
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
         <v>256</v>
       </c>
@@ -7753,7 +7753,7 @@
       <c r="I179" s="15"/>
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="11" t="s">
         <v>256</v>
       </c>
@@ -7781,7 +7781,7 @@
       <c r="I180" s="15"/>
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="11" t="s">
         <v>258</v>
       </c>
@@ -7807,7 +7807,7 @@
       <c r="I181" s="15"/>
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
         <v>258</v>
       </c>
@@ -7833,7 +7833,7 @@
       <c r="I182" s="15"/>
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
         <v>260</v>
       </c>
@@ -7861,7 +7861,7 @@
       <c r="I183" s="15"/>
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
         <v>264</v>
       </c>
@@ -7889,7 +7889,7 @@
       <c r="I184" s="15"/>
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
         <v>267</v>
       </c>
@@ -7917,7 +7917,7 @@
       <c r="I185" s="15"/>
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
         <v>311</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>422</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
         <v>271</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="21" customHeight="1">
+    <row r="189" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
         <v>273</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="11" t="s">
         <v>275</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="11" t="s">
         <v>277</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
         <v>277</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
         <v>279</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="11" t="s">
         <v>281</v>
       </c>
@@ -8194,70 +8194,6 @@
       <c r="J194" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="195" spans="1:10">
-      <c r="A195" s="1"/>
-      <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="1:10">
-      <c r="A196" s="1"/>
-      <c r="D196" s="1"/>
-    </row>
-    <row r="197" spans="1:10">
-      <c r="A197" s="1"/>
-      <c r="D197" s="1"/>
-    </row>
-    <row r="198" spans="1:10">
-      <c r="A198" s="1"/>
-      <c r="D198" s="1"/>
-    </row>
-    <row r="199" spans="1:10">
-      <c r="A199" s="1"/>
-      <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="1:10">
-      <c r="A200" s="1"/>
-      <c r="D200" s="1"/>
-    </row>
-    <row r="201" spans="1:10">
-      <c r="A201" s="1"/>
-      <c r="D201" s="1"/>
-    </row>
-    <row r="202" spans="1:10">
-      <c r="A202" s="1"/>
-      <c r="D202" s="1"/>
-    </row>
-    <row r="203" spans="1:10">
-      <c r="A203" s="1"/>
-      <c r="D203" s="1"/>
-    </row>
-    <row r="204" spans="1:10">
-      <c r="A204" s="1"/>
-      <c r="D204" s="1"/>
-    </row>
-    <row r="205" spans="1:10">
-      <c r="A205" s="1"/>
-      <c r="D205" s="1"/>
-    </row>
-    <row r="206" spans="1:10">
-      <c r="A206" s="1"/>
-      <c r="D206" s="1"/>
-    </row>
-    <row r="207" spans="1:10">
-      <c r="A207" s="1"/>
-      <c r="D207" s="1"/>
-    </row>
-    <row r="208" spans="1:10">
-      <c r="A208" s="1"/>
-      <c r="D208" s="1"/>
-    </row>
-    <row r="209" spans="1:4">
-      <c r="A209" s="1"/>
-      <c r="D209" s="1"/>
-    </row>
-    <row r="210" spans="1:4">
-      <c r="A210" s="1"/>
-      <c r="D210" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{E6C4BF4C-4228-4075-8FD7-3C862FC737BF}">

</xml_diff>